<commit_message>
fixed bug in model producing NaNs, updated food waste variable, and added soil management to docs
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E2E1C-5917-3640-A321-9C79DBBE8D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AD0AC1-4F8B-184A-9379-02E1ADE38986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="672">
   <si>
     <t>subsector</t>
   </si>
@@ -2050,6 +2050,9 @@
   <si>
     <t>ef_frst_forestfires_secondary_co2</t>
   </si>
+  <si>
+    <t>frac_agrc_agriculture_production_lost</t>
+  </si>
 </sst>
 </file>
 
@@ -2471,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS621"/>
+  <dimension ref="A1:AS622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A590" zoomScale="119" workbookViewId="0">
-      <selection activeCell="E611" sqref="E611"/>
+    <sheetView tabSelected="1" topLeftCell="A594" zoomScale="119" workbookViewId="0">
+      <selection activeCell="J615" sqref="J615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -77256,112 +77259,112 @@
         <v>1</v>
       </c>
       <c r="J612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="K612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="L612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="M612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="N612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="O612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="P612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="Q612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="R612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="S612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="T612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="U612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="V612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="W612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="X612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="Y612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="Z612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AA612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AB612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AC612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AD612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AE612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AF612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AG612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AH612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AI612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AJ612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AK612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AL612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AM612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AN612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AO612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AP612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AQ612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AR612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
       <c r="AS612">
-        <v>20</v>
+        <v>528.4</v>
       </c>
     </row>
     <row r="613" spans="1:45" x14ac:dyDescent="0.2">
@@ -78460,6 +78463,128 @@
       </c>
       <c r="AS621">
         <v>46.7</v>
+      </c>
+    </row>
+    <row r="622" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A622" t="s">
+        <v>45</v>
+      </c>
+      <c r="B622" t="s">
+        <v>671</v>
+      </c>
+      <c r="H622">
+        <v>0.86</v>
+      </c>
+      <c r="I622">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="K622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="L622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="M622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="N622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="O622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="P622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="Q622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="R622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="S622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="T622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="U622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="V622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="W622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="X622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="Y622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="Z622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AA622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AB622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AC622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AD622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AE622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AF622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AG622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AH622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AI622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AJ622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AK622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AL622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AM622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AN622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AO622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AP622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AQ622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AR622">
+        <v>0.21024000000000001</v>
+      </c>
+      <c r="AS622">
+        <v>0.21024000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scripts for generating transition probs
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA79AA1-DC24-7148-9F7E-4BF0A31DA9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA30B849-AAAC-D647-A430-27292AC9E379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6700" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -2437,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="AE230" zoomScale="119" workbookViewId="0">
+      <selection activeCell="AQ255" sqref="AQ255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33691,112 +33691,112 @@
         <v>1</v>
       </c>
       <c r="J256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="K256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="L256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="M256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="N256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="O256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="P256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="Q256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="R256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="S256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="T256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="U256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="V256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="W256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="X256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="Y256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="Z256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AA256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AB256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AC256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AD256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AE256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AF256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AG256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AH256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AI256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AJ256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AK256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AL256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AM256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AN256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AO256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AP256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AQ256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AR256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="AS256">
-        <v>1.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Some updates to transitions probabilities and data
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA30B849-AAAC-D647-A430-27292AC9E379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEDB9CA-0E1B-8C40-9392-9C09C57420B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6700" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2437,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE230" zoomScale="119" workbookViewId="0">
-      <selection activeCell="AQ255" sqref="AQ255"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3330,112 +3330,112 @@
         <v>1.2</v>
       </c>
       <c r="J8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="K8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="L8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="M8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="N8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="O8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="P8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="Q8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="R8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="S8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="T8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="U8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="V8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="W8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="X8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="Y8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="Z8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AA8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AB8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AC8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AD8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AE8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AF8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AG8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AH8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AI8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AJ8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AK8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AL8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AM8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AN8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AO8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AP8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AQ8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AR8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
       <c r="AS8">
-        <v>0.82</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.2">
@@ -3452,112 +3452,112 @@
         <v>1.2</v>
       </c>
       <c r="J9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="K9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="L9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="M9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="N9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="O9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="P9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Q9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="R9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="S9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="T9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="U9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="V9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="W9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="X9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Y9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Z9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AA9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AB9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AC9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AD9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AE9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AF9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AG9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AH9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AI9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AJ9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AK9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AL9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AM9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AN9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AO9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AP9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AQ9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AR9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AS9">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.2">
@@ -3574,112 +3574,112 @@
         <v>1.2</v>
       </c>
       <c r="J10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="K10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="L10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="M10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="N10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="O10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="P10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Q10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="R10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="S10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="T10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="U10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="V10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="W10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="X10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Y10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="Z10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AA10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AB10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AC10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AD10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AE10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AF10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AG10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AH10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AI10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AJ10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AK10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AL10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AM10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AN10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AO10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AP10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AQ10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AR10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="AS10">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
@@ -3696,112 +3696,112 @@
         <v>1.2</v>
       </c>
       <c r="J11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="K11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="V11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="W11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="X11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Y11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Z11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AA11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AB11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AC11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AD11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AF11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AG11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AI11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AJ11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AK11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AL11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AM11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AN11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AO11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AP11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AQ11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AR11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AS11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
@@ -3818,112 +3818,112 @@
         <v>1.2</v>
       </c>
       <c r="J12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="K12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="L12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="M12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="N12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="O12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="P12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="Q12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="R12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="S12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="T12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="U12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="V12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="W12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="X12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="Y12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="Z12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AA12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AB12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AC12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AD12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AE12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AF12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AG12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AH12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AI12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AJ12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AK12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AL12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AM12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AN12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AO12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AP12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AQ12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AR12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
       <c r="AS12">
-        <v>0.82</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
@@ -3940,112 +3940,112 @@
         <v>1.2</v>
       </c>
       <c r="J13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="K13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="V13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="X13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Y13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Z13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AA13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AB13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AC13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AD13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AF13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AG13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AI13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AJ13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AK13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AL13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AM13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AN13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AO13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AP13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AQ13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AR13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AS13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
@@ -4062,112 +4062,112 @@
         <v>1.2</v>
       </c>
       <c r="J14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="K14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="N14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="O14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="P14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="Q14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="R14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="T14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="U14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="V14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="W14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="X14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="Y14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="Z14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AA14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AB14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AC14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AD14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AE14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AF14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AG14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AH14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AI14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AJ14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AK14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AL14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AM14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AN14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AO14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AP14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AQ14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AR14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AS14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
@@ -4184,112 +4184,112 @@
         <v>1.2</v>
       </c>
       <c r="J15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="O15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="Q15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="R15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="T15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="U15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="V15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="W15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="X15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="Y15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="Z15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AA15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AB15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AC15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AE15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AF15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AG15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AH15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AI15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AJ15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AK15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AL15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AM15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AN15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AO15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AP15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AQ15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AR15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AS15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
@@ -4306,112 +4306,112 @@
         <v>1.2</v>
       </c>
       <c r="J16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="K16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="M16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="N16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="O16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="P16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="Q16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="R16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="S16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="T16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="U16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="V16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="W16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="X16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="Y16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="Z16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AA16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AB16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AC16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AD16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AE16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AF16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AG16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AH16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AI16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AJ16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AK16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AL16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AM16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AN16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AO16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AP16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AQ16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AR16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AS16">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
@@ -4428,112 +4428,112 @@
         <v>1.2</v>
       </c>
       <c r="J17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="L17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="M17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="O17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="P17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Q17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="R17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="S17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="T17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="U17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="V17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="W17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="X17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Y17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Z17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AA17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AB17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AC17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AD17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AE17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AF17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AG17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AH17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AI17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AJ17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AK17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AL17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AM17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AN17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AO17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AP17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AQ17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AR17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AS17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.2">
@@ -4550,112 +4550,112 @@
         <v>1.2</v>
       </c>
       <c r="J18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="K18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="L18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="M18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="N18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="O18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="P18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="Q18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="R18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="S18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="T18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="U18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="V18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="W18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="X18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="Y18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="Z18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AA18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AB18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AC18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AD18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AE18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AF18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AG18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AH18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AI18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AJ18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AK18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AL18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AM18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AN18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AO18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AP18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AQ18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AR18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="AS18">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.2">
@@ -4672,112 +4672,112 @@
         <v>1.2</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="K19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="V19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="W19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="X19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Y19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Z19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AA19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AB19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AC19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AD19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AF19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AG19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AI19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AJ19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AK19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AL19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AM19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AN19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AO19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AP19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AQ19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AR19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AS19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.2">
@@ -4794,112 +4794,112 @@
         <v>1.2</v>
       </c>
       <c r="J20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="K20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="O20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="X20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Y20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Z20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AA20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AB20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AC20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AD20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AF20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AG20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AI20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AJ20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AK20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AL20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AM20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AN20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AO20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AP20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AQ20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AR20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AS20">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.2">
@@ -11763,112 +11763,112 @@
         <v>1</v>
       </c>
       <c r="J77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="L77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="M77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="N77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="O77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="P77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Q77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="R77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="S77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="T77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="U77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="V77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="W77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="X77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Y77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AA77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AB77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AC77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AD77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AE77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AF77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AG77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AH77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AI77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AJ77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AK77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AL77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AM77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AN77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AO77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AP77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AQ77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AR77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AS77">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updted fake data 2
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6433FC96-4E6E-8C4E-9D3E-B7759C188767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356F8835-445C-F34D-878B-4682110E5F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="8020" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:AS609"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A499" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F525" sqref="F525"/>
+      <selection activeCell="E523" sqref="E523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated AFOLU to add fractional scalar for net imports/net exports implemented
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4679AF8-868F-DD44-A684-B202781C956F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426C2DA-9579-804C-A871-B37801F0EB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="8020" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="480" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="664">
   <si>
     <t>subsector</t>
   </si>
@@ -2014,6 +2014,21 @@
   <si>
     <t>frac_agrc_production_lost_sent_to_landfill</t>
   </si>
+  <si>
+    <t>frac_lndu_increasing_net_exports_met_croplands</t>
+  </si>
+  <si>
+    <t>frac_lndu_increasing_net_exports_met_grasslands</t>
+  </si>
+  <si>
+    <t>frac_lndu_proportion_grasslands_pasture</t>
+  </si>
+  <si>
+    <t>frac_lndu_increasing_net_imports_met_croplands</t>
+  </si>
+  <si>
+    <t>frac_lndu_increasing_net_imports_met_grasslands</t>
+  </si>
 </sst>
 </file>
 
@@ -2435,10 +2450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS609"/>
+  <dimension ref="A1:AS614"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" zoomScale="119" workbookViewId="0">
-      <selection activeCell="E523" sqref="E523"/>
+    <sheetView tabSelected="1" topLeftCell="A603" zoomScale="119" workbookViewId="0">
+      <selection activeCell="F612" sqref="F612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -76960,6 +76975,616 @@
       </c>
       <c r="AS609">
         <v>10</v>
+      </c>
+    </row>
+    <row r="610" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A610" t="s">
+        <v>47</v>
+      </c>
+      <c r="B610" t="s">
+        <v>659</v>
+      </c>
+      <c r="H610">
+        <v>1</v>
+      </c>
+      <c r="I610">
+        <v>1</v>
+      </c>
+      <c r="J610">
+        <v>1</v>
+      </c>
+      <c r="K610">
+        <v>1</v>
+      </c>
+      <c r="L610">
+        <v>1</v>
+      </c>
+      <c r="M610">
+        <v>1</v>
+      </c>
+      <c r="N610">
+        <v>1</v>
+      </c>
+      <c r="O610">
+        <v>1</v>
+      </c>
+      <c r="P610">
+        <v>1</v>
+      </c>
+      <c r="Q610">
+        <v>1</v>
+      </c>
+      <c r="R610">
+        <v>1</v>
+      </c>
+      <c r="S610">
+        <v>1</v>
+      </c>
+      <c r="T610">
+        <v>1</v>
+      </c>
+      <c r="U610">
+        <v>1</v>
+      </c>
+      <c r="V610">
+        <v>1</v>
+      </c>
+      <c r="W610">
+        <v>1</v>
+      </c>
+      <c r="X610">
+        <v>1</v>
+      </c>
+      <c r="Y610">
+        <v>1</v>
+      </c>
+      <c r="Z610">
+        <v>1</v>
+      </c>
+      <c r="AA610">
+        <v>1</v>
+      </c>
+      <c r="AB610">
+        <v>1</v>
+      </c>
+      <c r="AC610">
+        <v>1</v>
+      </c>
+      <c r="AD610">
+        <v>1</v>
+      </c>
+      <c r="AE610">
+        <v>1</v>
+      </c>
+      <c r="AF610">
+        <v>1</v>
+      </c>
+      <c r="AG610">
+        <v>1</v>
+      </c>
+      <c r="AH610">
+        <v>1</v>
+      </c>
+      <c r="AI610">
+        <v>1</v>
+      </c>
+      <c r="AJ610">
+        <v>1</v>
+      </c>
+      <c r="AK610">
+        <v>1</v>
+      </c>
+      <c r="AL610">
+        <v>1</v>
+      </c>
+      <c r="AM610">
+        <v>1</v>
+      </c>
+      <c r="AN610">
+        <v>1</v>
+      </c>
+      <c r="AO610">
+        <v>1</v>
+      </c>
+      <c r="AP610">
+        <v>1</v>
+      </c>
+      <c r="AQ610">
+        <v>1</v>
+      </c>
+      <c r="AR610">
+        <v>1</v>
+      </c>
+      <c r="AS610">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A611" t="s">
+        <v>47</v>
+      </c>
+      <c r="B611" t="s">
+        <v>660</v>
+      </c>
+      <c r="H611">
+        <v>1</v>
+      </c>
+      <c r="I611">
+        <v>1</v>
+      </c>
+      <c r="J611">
+        <v>1</v>
+      </c>
+      <c r="K611">
+        <v>1</v>
+      </c>
+      <c r="L611">
+        <v>1</v>
+      </c>
+      <c r="M611">
+        <v>1</v>
+      </c>
+      <c r="N611">
+        <v>1</v>
+      </c>
+      <c r="O611">
+        <v>1</v>
+      </c>
+      <c r="P611">
+        <v>1</v>
+      </c>
+      <c r="Q611">
+        <v>1</v>
+      </c>
+      <c r="R611">
+        <v>1</v>
+      </c>
+      <c r="S611">
+        <v>1</v>
+      </c>
+      <c r="T611">
+        <v>1</v>
+      </c>
+      <c r="U611">
+        <v>1</v>
+      </c>
+      <c r="V611">
+        <v>1</v>
+      </c>
+      <c r="W611">
+        <v>1</v>
+      </c>
+      <c r="X611">
+        <v>1</v>
+      </c>
+      <c r="Y611">
+        <v>1</v>
+      </c>
+      <c r="Z611">
+        <v>1</v>
+      </c>
+      <c r="AA611">
+        <v>1</v>
+      </c>
+      <c r="AB611">
+        <v>1</v>
+      </c>
+      <c r="AC611">
+        <v>1</v>
+      </c>
+      <c r="AD611">
+        <v>1</v>
+      </c>
+      <c r="AE611">
+        <v>1</v>
+      </c>
+      <c r="AF611">
+        <v>1</v>
+      </c>
+      <c r="AG611">
+        <v>1</v>
+      </c>
+      <c r="AH611">
+        <v>1</v>
+      </c>
+      <c r="AI611">
+        <v>1</v>
+      </c>
+      <c r="AJ611">
+        <v>1</v>
+      </c>
+      <c r="AK611">
+        <v>1</v>
+      </c>
+      <c r="AL611">
+        <v>1</v>
+      </c>
+      <c r="AM611">
+        <v>1</v>
+      </c>
+      <c r="AN611">
+        <v>1</v>
+      </c>
+      <c r="AO611">
+        <v>1</v>
+      </c>
+      <c r="AP611">
+        <v>1</v>
+      </c>
+      <c r="AQ611">
+        <v>1</v>
+      </c>
+      <c r="AR611">
+        <v>1</v>
+      </c>
+      <c r="AS611">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="612" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A612" t="s">
+        <v>47</v>
+      </c>
+      <c r="B612" t="s">
+        <v>661</v>
+      </c>
+      <c r="H612">
+        <v>1</v>
+      </c>
+      <c r="I612">
+        <v>1</v>
+      </c>
+      <c r="J612">
+        <v>0.4</v>
+      </c>
+      <c r="K612">
+        <v>0.4</v>
+      </c>
+      <c r="L612">
+        <v>0.4</v>
+      </c>
+      <c r="M612">
+        <v>0.4</v>
+      </c>
+      <c r="N612">
+        <v>0.4</v>
+      </c>
+      <c r="O612">
+        <v>0.4</v>
+      </c>
+      <c r="P612">
+        <v>0.4</v>
+      </c>
+      <c r="Q612">
+        <v>0.4</v>
+      </c>
+      <c r="R612">
+        <v>0.4</v>
+      </c>
+      <c r="S612">
+        <v>0.4</v>
+      </c>
+      <c r="T612">
+        <v>0.4</v>
+      </c>
+      <c r="U612">
+        <v>0.4</v>
+      </c>
+      <c r="V612">
+        <v>0.4</v>
+      </c>
+      <c r="W612">
+        <v>0.4</v>
+      </c>
+      <c r="X612">
+        <v>0.4</v>
+      </c>
+      <c r="Y612">
+        <v>0.4</v>
+      </c>
+      <c r="Z612">
+        <v>0.4</v>
+      </c>
+      <c r="AA612">
+        <v>0.4</v>
+      </c>
+      <c r="AB612">
+        <v>0.4</v>
+      </c>
+      <c r="AC612">
+        <v>0.4</v>
+      </c>
+      <c r="AD612">
+        <v>0.4</v>
+      </c>
+      <c r="AE612">
+        <v>0.4</v>
+      </c>
+      <c r="AF612">
+        <v>0.4</v>
+      </c>
+      <c r="AG612">
+        <v>0.4</v>
+      </c>
+      <c r="AH612">
+        <v>0.4</v>
+      </c>
+      <c r="AI612">
+        <v>0.4</v>
+      </c>
+      <c r="AJ612">
+        <v>0.4</v>
+      </c>
+      <c r="AK612">
+        <v>0.4</v>
+      </c>
+      <c r="AL612">
+        <v>0.4</v>
+      </c>
+      <c r="AM612">
+        <v>0.4</v>
+      </c>
+      <c r="AN612">
+        <v>0.4</v>
+      </c>
+      <c r="AO612">
+        <v>0.4</v>
+      </c>
+      <c r="AP612">
+        <v>0.4</v>
+      </c>
+      <c r="AQ612">
+        <v>0.4</v>
+      </c>
+      <c r="AR612">
+        <v>0.4</v>
+      </c>
+      <c r="AS612">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="613" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A613" t="s">
+        <v>47</v>
+      </c>
+      <c r="B613" t="s">
+        <v>662</v>
+      </c>
+      <c r="H613">
+        <v>1</v>
+      </c>
+      <c r="I613">
+        <v>1</v>
+      </c>
+      <c r="J613">
+        <v>1</v>
+      </c>
+      <c r="K613">
+        <v>1</v>
+      </c>
+      <c r="L613">
+        <v>1</v>
+      </c>
+      <c r="M613">
+        <v>1</v>
+      </c>
+      <c r="N613">
+        <v>1</v>
+      </c>
+      <c r="O613">
+        <v>1</v>
+      </c>
+      <c r="P613">
+        <v>1</v>
+      </c>
+      <c r="Q613">
+        <v>1</v>
+      </c>
+      <c r="R613">
+        <v>1</v>
+      </c>
+      <c r="S613">
+        <v>1</v>
+      </c>
+      <c r="T613">
+        <v>1</v>
+      </c>
+      <c r="U613">
+        <v>1</v>
+      </c>
+      <c r="V613">
+        <v>1</v>
+      </c>
+      <c r="W613">
+        <v>1</v>
+      </c>
+      <c r="X613">
+        <v>1</v>
+      </c>
+      <c r="Y613">
+        <v>1</v>
+      </c>
+      <c r="Z613">
+        <v>1</v>
+      </c>
+      <c r="AA613">
+        <v>1</v>
+      </c>
+      <c r="AB613">
+        <v>1</v>
+      </c>
+      <c r="AC613">
+        <v>1</v>
+      </c>
+      <c r="AD613">
+        <v>1</v>
+      </c>
+      <c r="AE613">
+        <v>1</v>
+      </c>
+      <c r="AF613">
+        <v>1</v>
+      </c>
+      <c r="AG613">
+        <v>1</v>
+      </c>
+      <c r="AH613">
+        <v>1</v>
+      </c>
+      <c r="AI613">
+        <v>1</v>
+      </c>
+      <c r="AJ613">
+        <v>1</v>
+      </c>
+      <c r="AK613">
+        <v>1</v>
+      </c>
+      <c r="AL613">
+        <v>1</v>
+      </c>
+      <c r="AM613">
+        <v>1</v>
+      </c>
+      <c r="AN613">
+        <v>1</v>
+      </c>
+      <c r="AO613">
+        <v>1</v>
+      </c>
+      <c r="AP613">
+        <v>1</v>
+      </c>
+      <c r="AQ613">
+        <v>1</v>
+      </c>
+      <c r="AR613">
+        <v>1</v>
+      </c>
+      <c r="AS613">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="614" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A614" t="s">
+        <v>47</v>
+      </c>
+      <c r="B614" t="s">
+        <v>663</v>
+      </c>
+      <c r="H614">
+        <v>1</v>
+      </c>
+      <c r="I614">
+        <v>1</v>
+      </c>
+      <c r="J614">
+        <v>1</v>
+      </c>
+      <c r="K614">
+        <v>1</v>
+      </c>
+      <c r="L614">
+        <v>1</v>
+      </c>
+      <c r="M614">
+        <v>1</v>
+      </c>
+      <c r="N614">
+        <v>1</v>
+      </c>
+      <c r="O614">
+        <v>1</v>
+      </c>
+      <c r="P614">
+        <v>1</v>
+      </c>
+      <c r="Q614">
+        <v>1</v>
+      </c>
+      <c r="R614">
+        <v>1</v>
+      </c>
+      <c r="S614">
+        <v>1</v>
+      </c>
+      <c r="T614">
+        <v>1</v>
+      </c>
+      <c r="U614">
+        <v>1</v>
+      </c>
+      <c r="V614">
+        <v>1</v>
+      </c>
+      <c r="W614">
+        <v>1</v>
+      </c>
+      <c r="X614">
+        <v>1</v>
+      </c>
+      <c r="Y614">
+        <v>1</v>
+      </c>
+      <c r="Z614">
+        <v>1</v>
+      </c>
+      <c r="AA614">
+        <v>1</v>
+      </c>
+      <c r="AB614">
+        <v>1</v>
+      </c>
+      <c r="AC614">
+        <v>1</v>
+      </c>
+      <c r="AD614">
+        <v>1</v>
+      </c>
+      <c r="AE614">
+        <v>1</v>
+      </c>
+      <c r="AF614">
+        <v>1</v>
+      </c>
+      <c r="AG614">
+        <v>1</v>
+      </c>
+      <c r="AH614">
+        <v>1</v>
+      </c>
+      <c r="AI614">
+        <v>1</v>
+      </c>
+      <c r="AJ614">
+        <v>1</v>
+      </c>
+      <c r="AK614">
+        <v>1</v>
+      </c>
+      <c r="AL614">
+        <v>1</v>
+      </c>
+      <c r="AM614">
+        <v>1</v>
+      </c>
+      <c r="AN614">
+        <v>1</v>
+      </c>
+      <c r="AO614">
+        <v>1</v>
+      </c>
+      <c r="AP614">
+        <v>1</v>
+      </c>
+      <c r="AQ614">
+        <v>1</v>
+      </c>
+      <c r="AR614">
+        <v>1</v>
+      </c>
+      <c r="AS614">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated model to fix demand and population outputs, improve reallocatin, and add pasture fraction of grassland
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426C2DA-9579-804C-A871-B37801F0EB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6E0104-273D-D749-841A-1F030B5D7FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6660" yWindow="480" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2453,7 +2453,7 @@
   <dimension ref="A1:AS614"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A603" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F612" sqref="F612"/>
+      <selection activeCell="B609" sqref="B609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated sampling units and continued work towards uncertainty structuring
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE57217-A6DE-FC41-AE49-FFADD6637828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AACEC92-5CF4-294C-9D90-61FC492BD024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8920" yWindow="460" windowWidth="22140" windowHeight="20600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="715">
   <si>
     <t>subsector</t>
   </si>
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS665"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B578" zoomScale="119" workbookViewId="0">
-      <selection activeCell="B601" sqref="B601"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2662,8 +2662,8 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
+      <c r="N1" s="1">
+        <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -83978,10 +83978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -84123,6 +84123,128 @@
         <v>44</v>
       </c>
     </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2">
+        <v>0.6</v>
+      </c>
+      <c r="I2">
+        <v>1.74</v>
+      </c>
+      <c r="J2">
+        <v>157.47999999999999</v>
+      </c>
+      <c r="K2">
+        <v>157.47999999999999</v>
+      </c>
+      <c r="L2">
+        <v>155.47999999999999</v>
+      </c>
+      <c r="M2">
+        <v>153.47999999999999</v>
+      </c>
+      <c r="N2">
+        <v>151.47999999999999</v>
+      </c>
+      <c r="O2">
+        <v>149.47999999999999</v>
+      </c>
+      <c r="P2">
+        <v>147.47999999999999</v>
+      </c>
+      <c r="Q2">
+        <v>145.47999999999999</v>
+      </c>
+      <c r="R2">
+        <v>143.47999999999999</v>
+      </c>
+      <c r="S2">
+        <v>141.47999999999999</v>
+      </c>
+      <c r="T2">
+        <v>139.47999999999999</v>
+      </c>
+      <c r="U2">
+        <v>137.47999999999999</v>
+      </c>
+      <c r="V2">
+        <v>135.47999999999999</v>
+      </c>
+      <c r="W2">
+        <v>133.47999999999999</v>
+      </c>
+      <c r="X2">
+        <v>131.47999999999999</v>
+      </c>
+      <c r="Y2">
+        <v>129.47999999999999</v>
+      </c>
+      <c r="Z2">
+        <v>127.48</v>
+      </c>
+      <c r="AA2">
+        <v>125.48</v>
+      </c>
+      <c r="AB2">
+        <v>123.48</v>
+      </c>
+      <c r="AC2">
+        <v>121.48</v>
+      </c>
+      <c r="AD2">
+        <v>119.48</v>
+      </c>
+      <c r="AE2">
+        <v>117.48</v>
+      </c>
+      <c r="AF2">
+        <v>115.48</v>
+      </c>
+      <c r="AG2">
+        <v>113.48</v>
+      </c>
+      <c r="AH2">
+        <v>111.48</v>
+      </c>
+      <c r="AI2">
+        <v>109.48</v>
+      </c>
+      <c r="AJ2">
+        <v>107.48</v>
+      </c>
+      <c r="AK2">
+        <v>105.48</v>
+      </c>
+      <c r="AL2">
+        <v>103.48</v>
+      </c>
+      <c r="AM2">
+        <v>101.48</v>
+      </c>
+      <c r="AN2">
+        <v>99.48</v>
+      </c>
+      <c r="AO2">
+        <v>97.48</v>
+      </c>
+      <c r="AP2">
+        <v>95.48</v>
+      </c>
+      <c r="AQ2">
+        <v>93.48</v>
+      </c>
+      <c r="AR2">
+        <v>91.48</v>
+      </c>
+      <c r="AS2">
+        <v>89.48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>